<commit_message>
new psa data format
</commit_message>
<xml_diff>
--- a/inputs/PSA_materials.xlsx
+++ b/inputs/PSA_materials.xlsx
@@ -277,40 +277,40 @@
     <t>Zamboanga Sibugay</t>
   </si>
   <si>
-    <t>PropRoof_Strong material(galvanized,iron,al,tile,concrete,brick,stone,asbestos)</t>
+    <t>Roof_Strong material(galvanized,iron,al,tile,concrete,brick,stone,asbestos)</t>
   </si>
   <si>
-    <t>PropRoof_Light material</t>
+    <t>Roof_Light material</t>
   </si>
   <si>
-    <t>PropRoof_Salvaged/makeshift materials</t>
+    <t>Roof_Salvaged/makeshift materials</t>
   </si>
   <si>
-    <t>PropRoof_Mixed but predominantly strong materials</t>
+    <t>Roof_Mixed but predominantly strong materials</t>
   </si>
   <si>
-    <t>PropRoof_Mixed but predominantly light materials</t>
+    <t>Roof_Mixed but predominantly light materials</t>
   </si>
   <si>
-    <t>PropRoof_Mixed but predominantly salvaged materials</t>
+    <t>Roof_Mixed but predominantly salvaged materials</t>
   </si>
   <si>
-    <t>PropWall_Strong material(galvanized,iron,al,tile,concrete,brick,stone,asbestos)</t>
+    <t>Wall_Strong material(galvanized,iron,al,tile,concrete,brick,stone,asbestos)</t>
   </si>
   <si>
-    <t>PropWall_Light material</t>
+    <t>Wall_Light material</t>
   </si>
   <si>
-    <t>PropWall_Salvaged/makeshift materials</t>
+    <t>Wall_Salvaged/makeshift materials</t>
   </si>
   <si>
-    <t>PropWall_Mixed but predominantly strong materials</t>
+    <t>Wall_Mixed but predominantly strong materials</t>
   </si>
   <si>
-    <t>PropWall_Mixed but predominantly light materials</t>
+    <t>Wall_Mixed but predominantly light materials</t>
   </si>
   <si>
-    <t>PropWall_Mixed but predominantly salvaged materials</t>
+    <t>Wall_Mixed but predominantly salvaged materials</t>
   </si>
 </sst>
 </file>
@@ -7757,7 +7757,7 @@
   <dimension ref="A1:G87"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>